<commit_message>
read me file changes
</commit_message>
<xml_diff>
--- a/UHI Submission Sheet- Innovation Track.xlsx
+++ b/UHI Submission Sheet- Innovation Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kishorepujari/UHI_Innovation_challenge_1_OracleCerner_Final_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA314B7-6E34-8045-B579-5B8723DEEB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F290CB8-8F1B-6A48-ABF1-53140710DEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -228,6 +228,9 @@
   </si>
   <si>
     <t>We have resued handwriting and speech to text features from android</t>
+  </si>
+  <si>
+    <t>Due to time restrictions we have just hard coded the API_KEY, this can further enahnced to oauth or JWT token type of mechanisms</t>
   </si>
 </sst>
 </file>
@@ -964,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:AG1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15:G21"/>
+    <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1299,7 +1302,7 @@
         <v>55</v>
       </c>
       <c r="M8" s="35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="N8" s="35" t="s">
         <v>59</v>
@@ -2637,7 +2640,7 @@
       <c r="AF41" s="18"/>
       <c r="AG41" s="18"/>
     </row>
-    <row r="42" spans="1:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:33" ht="38" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="32"/>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>

</xml_diff>

<commit_message>
Modified UI screens and code
</commit_message>
<xml_diff>
--- a/UHI Submission Sheet- Innovation Track.xlsx
+++ b/UHI Submission Sheet- Innovation Track.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kishorepujari/UHI_Innovation_challenge_1_OracleCerner_Final_submission/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58E69A57-263D-CB48-9609-F0F74E577172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E805EF72-0AA9-644A-928E-42EDF609525B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35840" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,13 +224,13 @@
     <t>Due to time restrictions we have just hard coded the API_KEY, this can further enahnced to oauth or JWT type of mechanisms</t>
   </si>
   <si>
-    <t>Language translation has been done but due to lack time we couldn't  integrate it in the apps</t>
-  </si>
-  <si>
     <t>We have resued handwriting and speech to text features from android</t>
   </si>
   <si>
     <t>Due to time restrictions we have just hard coded the API_KEY, this can further enahnced to oauth or JWT token type of mechanisms</t>
+  </si>
+  <si>
+    <t>Language translation can be demoed from local host</t>
   </si>
 </sst>
 </file>
@@ -669,25 +669,14 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -696,9 +685,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -967,8 +967,8 @@
   </sheetPr>
   <dimension ref="A1:AG1042"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="223" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+    <sheetView tabSelected="1" topLeftCell="J25" zoomScale="223" workbookViewId="0">
+      <selection activeCell="N39" sqref="N39:N42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -982,22 +982,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="19" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="37"/>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="38"/>
+      <c r="B1" s="44"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44"/>
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="N1" s="45"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -1018,7 +1018,7 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:33" ht="14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:33" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -1092,7 +1092,7 @@
       <c r="AF3" s="13"/>
       <c r="AG3" s="13"/>
     </row>
-    <row r="4" spans="1:33" ht="14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="14"/>
       <c r="B4" s="9" t="s">
         <v>2</v>
@@ -1134,7 +1134,7 @@
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="45" t="s">
+      <c r="C5" s="30" t="s">
         <v>50</v>
       </c>
       <c r="D5" s="15"/>
@@ -1265,13 +1265,13 @@
       <c r="AG7" s="24"/>
     </row>
     <row r="8" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="30">
+      <c r="A8" s="40">
         <v>1</v>
       </c>
-      <c r="B8" s="33" t="s">
+      <c r="B8" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="42" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="25" t="s">
@@ -1283,29 +1283,29 @@
       <c r="F8" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="K8" s="35" t="s">
+      <c r="K8" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="L8" s="35" t="s">
+      <c r="L8" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="M8" s="35" t="s">
+      <c r="M8" s="31" t="s">
+        <v>60</v>
+      </c>
+      <c r="N8" s="31" t="s">
         <v>61</v>
-      </c>
-      <c r="N8" s="35" t="s">
-        <v>59</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="18"/>
@@ -1328,9 +1328,9 @@
       <c r="AG8" s="18"/>
     </row>
     <row r="9" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="31"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
       <c r="D9" s="25" t="s">
         <v>21</v>
       </c>
@@ -1340,14 +1340,14 @@
       <c r="F9" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="L9" s="31"/>
-      <c r="M9" s="31"/>
-      <c r="N9" s="31"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+      <c r="L9" s="32"/>
+      <c r="M9" s="32"/>
+      <c r="N9" s="32"/>
       <c r="O9" s="18"/>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
@@ -1369,9 +1369,9 @@
       <c r="AG9" s="18"/>
     </row>
     <row r="10" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="31"/>
-      <c r="B10" s="31"/>
-      <c r="C10" s="31"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
       <c r="D10" s="25" t="s">
         <v>22</v>
       </c>
@@ -1381,14 +1381,14 @@
       <c r="F10" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="31"/>
-      <c r="K10" s="31"/>
-      <c r="L10" s="31"/>
-      <c r="M10" s="31"/>
-      <c r="N10" s="31"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="32"/>
+      <c r="N10" s="32"/>
       <c r="O10" s="18"/>
       <c r="P10" s="18"/>
       <c r="Q10" s="18"/>
@@ -1410,9 +1410,9 @@
       <c r="AG10" s="18"/>
     </row>
     <row r="11" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="31"/>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
       <c r="D11" s="25" t="s">
         <v>23</v>
       </c>
@@ -1422,14 +1422,14 @@
       <c r="F11" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31"/>
-      <c r="K11" s="31"/>
-      <c r="L11" s="31"/>
-      <c r="M11" s="31"/>
-      <c r="N11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
+      <c r="M11" s="32"/>
+      <c r="N11" s="32"/>
       <c r="O11" s="18"/>
       <c r="P11" s="18"/>
       <c r="Q11" s="18"/>
@@ -1451,9 +1451,9 @@
       <c r="AG11" s="18"/>
     </row>
     <row r="12" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="31"/>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
       <c r="D12" s="25" t="s">
         <v>24</v>
       </c>
@@ -1463,14 +1463,14 @@
       <c r="F12" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="32"/>
+      <c r="N12" s="32"/>
       <c r="O12" s="18"/>
       <c r="P12" s="18"/>
       <c r="Q12" s="18"/>
@@ -1492,9 +1492,9 @@
       <c r="AG12" s="18"/>
     </row>
     <row r="13" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="32"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
       <c r="D13" s="25" t="s">
         <v>26</v>
       </c>
@@ -1504,14 +1504,14 @@
       <c r="F13" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="33"/>
       <c r="O13" s="18"/>
       <c r="P13" s="18"/>
       <c r="Q13" s="18"/>
@@ -1568,13 +1568,13 @@
       <c r="AG14" s="18"/>
     </row>
     <row r="15" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A15" s="30">
+      <c r="A15" s="40">
         <v>2</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="42" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="25" t="s">
@@ -1584,14 +1584,14 @@
         <v>20</v>
       </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
+      <c r="L15" s="31"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="31"/>
       <c r="O15" s="18"/>
       <c r="P15" s="18"/>
       <c r="Q15" s="18"/>
@@ -1613,9 +1613,9 @@
       <c r="AG15" s="18"/>
     </row>
     <row r="16" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A16" s="31"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
       <c r="D16" s="25" t="s">
         <v>21</v>
       </c>
@@ -1623,14 +1623,14 @@
         <v>20</v>
       </c>
       <c r="F16" s="29"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
-      <c r="J16" s="31"/>
-      <c r="K16" s="31"/>
-      <c r="L16" s="31"/>
-      <c r="M16" s="31"/>
-      <c r="N16" s="31"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="32"/>
+      <c r="N16" s="32"/>
       <c r="O16" s="18"/>
       <c r="P16" s="18"/>
       <c r="Q16" s="18"/>
@@ -1652,9 +1652,9 @@
       <c r="AG16" s="18"/>
     </row>
     <row r="17" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A17" s="31"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="32"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="25" t="s">
         <v>22</v>
       </c>
@@ -1662,14 +1662,14 @@
         <v>20</v>
       </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31"/>
-      <c r="K17" s="31"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="32"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="32"/>
       <c r="O17" s="18"/>
       <c r="P17" s="18"/>
       <c r="Q17" s="18"/>
@@ -1691,9 +1691,9 @@
       <c r="AG17" s="18"/>
     </row>
     <row r="18" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="25" t="s">
         <v>23</v>
       </c>
@@ -1701,14 +1701,14 @@
         <v>20</v>
       </c>
       <c r="F18" s="29"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
-      <c r="J18" s="31"/>
-      <c r="K18" s="31"/>
-      <c r="L18" s="31"/>
-      <c r="M18" s="31"/>
-      <c r="N18" s="31"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="32"/>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
       <c r="O18" s="18"/>
       <c r="P18" s="18"/>
       <c r="Q18" s="18"/>
@@ -1730,9 +1730,9 @@
       <c r="AG18" s="18"/>
     </row>
     <row r="19" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A19" s="31"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
       <c r="D19" s="25" t="s">
         <v>24</v>
       </c>
@@ -1740,14 +1740,14 @@
         <v>20</v>
       </c>
       <c r="F19" s="29"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
-      <c r="J19" s="31"/>
-      <c r="K19" s="31"/>
-      <c r="L19" s="31"/>
-      <c r="M19" s="31"/>
-      <c r="N19" s="31"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
       <c r="O19" s="18"/>
       <c r="P19" s="18"/>
       <c r="Q19" s="18"/>
@@ -1769,9 +1769,9 @@
       <c r="AG19" s="18"/>
     </row>
     <row r="20" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A20" s="32"/>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
       <c r="D20" s="25" t="s">
         <v>26</v>
       </c>
@@ -1779,14 +1779,14 @@
         <v>25</v>
       </c>
       <c r="F20" s="29"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="31"/>
-      <c r="M20" s="31"/>
-      <c r="N20" s="31"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
       <c r="O20" s="18"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
@@ -1809,8 +1809,8 @@
     </row>
     <row r="21" spans="1:33" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="27"/>
-      <c r="B21" s="31"/>
-      <c r="C21" s="31"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
       <c r="D21" s="25" t="s">
         <v>29</v>
       </c>
@@ -1818,14 +1818,14 @@
         <v>25</v>
       </c>
       <c r="F21" s="29"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="33"/>
+      <c r="M21" s="33"/>
+      <c r="N21" s="33"/>
       <c r="O21" s="18"/>
       <c r="P21" s="18"/>
       <c r="Q21" s="18"/>
@@ -1848,8 +1848,8 @@
     </row>
     <row r="22" spans="1:33" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="27"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="17"/>
@@ -1917,13 +1917,13 @@
       <c r="AG23" s="18"/>
     </row>
     <row r="24" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A24" s="30">
+      <c r="A24" s="40">
         <v>3</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="42" t="s">
         <v>31</v>
       </c>
       <c r="D24" s="25" t="s">
@@ -1933,14 +1933,14 @@
         <v>20</v>
       </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="35"/>
-      <c r="N24" s="35"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
+      <c r="I24" s="31"/>
+      <c r="J24" s="31"/>
+      <c r="K24" s="31"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="31"/>
       <c r="O24" s="18"/>
       <c r="P24" s="18"/>
       <c r="Q24" s="18"/>
@@ -1962,9 +1962,9 @@
       <c r="AG24" s="18"/>
     </row>
     <row r="25" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A25" s="31"/>
-      <c r="B25" s="31"/>
-      <c r="C25" s="31"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="25" t="s">
         <v>21</v>
       </c>
@@ -1972,14 +1972,14 @@
         <v>20</v>
       </c>
       <c r="F25" s="29"/>
-      <c r="G25" s="31"/>
-      <c r="H25" s="31"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
-      <c r="M25" s="31"/>
-      <c r="N25" s="31"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
       <c r="O25" s="18"/>
       <c r="P25" s="18"/>
       <c r="Q25" s="18"/>
@@ -2001,9 +2001,9 @@
       <c r="AG25" s="18"/>
     </row>
     <row r="26" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A26" s="31"/>
-      <c r="B26" s="31"/>
-      <c r="C26" s="31"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="25" t="s">
         <v>22</v>
       </c>
@@ -2011,14 +2011,14 @@
         <v>20</v>
       </c>
       <c r="F26" s="29"/>
-      <c r="G26" s="31"/>
-      <c r="H26" s="31"/>
-      <c r="I26" s="31"/>
-      <c r="J26" s="31"/>
-      <c r="K26" s="31"/>
-      <c r="L26" s="31"/>
-      <c r="M26" s="31"/>
-      <c r="N26" s="31"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
       <c r="O26" s="18"/>
       <c r="P26" s="18"/>
       <c r="Q26" s="18"/>
@@ -2040,9 +2040,9 @@
       <c r="AG26" s="18"/>
     </row>
     <row r="27" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A27" s="31"/>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
       <c r="D27" s="25" t="s">
         <v>23</v>
       </c>
@@ -2050,14 +2050,14 @@
         <v>20</v>
       </c>
       <c r="F27" s="29"/>
-      <c r="G27" s="31"/>
-      <c r="H27" s="31"/>
-      <c r="I27" s="31"/>
-      <c r="J27" s="31"/>
-      <c r="K27" s="31"/>
-      <c r="L27" s="31"/>
-      <c r="M27" s="31"/>
-      <c r="N27" s="31"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="32"/>
+      <c r="N27" s="32"/>
       <c r="O27" s="18"/>
       <c r="P27" s="18"/>
       <c r="Q27" s="18"/>
@@ -2079,9 +2079,9 @@
       <c r="AG27" s="18"/>
     </row>
     <row r="28" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A28" s="31"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
       <c r="D28" s="25" t="s">
         <v>24</v>
       </c>
@@ -2089,14 +2089,14 @@
         <v>20</v>
       </c>
       <c r="F28" s="29"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="31"/>
-      <c r="I28" s="31"/>
-      <c r="J28" s="31"/>
-      <c r="K28" s="31"/>
-      <c r="L28" s="31"/>
-      <c r="M28" s="31"/>
-      <c r="N28" s="31"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
       <c r="O28" s="18"/>
       <c r="P28" s="18"/>
       <c r="Q28" s="18"/>
@@ -2118,9 +2118,9 @@
       <c r="AG28" s="18"/>
     </row>
     <row r="29" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="31"/>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
       <c r="D29" s="25" t="s">
         <v>26</v>
       </c>
@@ -2128,14 +2128,14 @@
         <v>25</v>
       </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
+      <c r="G29" s="32"/>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32"/>
+      <c r="K29" s="32"/>
+      <c r="L29" s="32"/>
+      <c r="M29" s="32"/>
+      <c r="N29" s="32"/>
       <c r="O29" s="18"/>
       <c r="P29" s="18"/>
       <c r="Q29" s="18"/>
@@ -2157,9 +2157,9 @@
       <c r="AG29" s="18"/>
     </row>
     <row r="30" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="32"/>
+      <c r="A30" s="33"/>
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
       <c r="D30" s="25" t="s">
         <v>29</v>
       </c>
@@ -2167,14 +2167,14 @@
         <v>25</v>
       </c>
       <c r="F30" s="29"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
-      <c r="I30" s="32"/>
-      <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-      <c r="M30" s="32"/>
-      <c r="N30" s="32"/>
+      <c r="G30" s="33"/>
+      <c r="H30" s="33"/>
+      <c r="I30" s="33"/>
+      <c r="J30" s="33"/>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="33"/>
       <c r="O30" s="18"/>
       <c r="P30" s="18"/>
       <c r="Q30" s="18"/>
@@ -2231,13 +2231,13 @@
       <c r="AG31" s="18"/>
     </row>
     <row r="32" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A32" s="30">
+      <c r="A32" s="40">
         <v>4</v>
       </c>
-      <c r="B32" s="33" t="s">
+      <c r="B32" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C32" s="34" t="s">
+      <c r="C32" s="42" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="25" t="s">
@@ -2247,14 +2247,14 @@
         <v>20</v>
       </c>
       <c r="F32" s="29"/>
-      <c r="G32" s="35"/>
-      <c r="H32" s="35"/>
-      <c r="I32" s="35"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
       <c r="O32" s="18"/>
       <c r="P32" s="18"/>
       <c r="Q32" s="18"/>
@@ -2276,9 +2276,9 @@
       <c r="AG32" s="18"/>
     </row>
     <row r="33" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A33" s="31"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
       <c r="D33" s="25" t="s">
         <v>21</v>
       </c>
@@ -2286,14 +2286,14 @@
         <v>20</v>
       </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="31"/>
-      <c r="N33" s="31"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32"/>
+      <c r="N33" s="32"/>
       <c r="O33" s="18"/>
       <c r="P33" s="18"/>
       <c r="Q33" s="18"/>
@@ -2315,9 +2315,9 @@
       <c r="AG33" s="18"/>
     </row>
     <row r="34" spans="1:33" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="31"/>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
       <c r="D34" s="25" t="s">
         <v>22</v>
       </c>
@@ -2325,14 +2325,14 @@
         <v>20</v>
       </c>
       <c r="F34" s="29"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="31"/>
-      <c r="N34" s="31"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="32"/>
+      <c r="J34" s="32"/>
+      <c r="K34" s="32"/>
+      <c r="L34" s="32"/>
+      <c r="M34" s="32"/>
+      <c r="N34" s="32"/>
       <c r="O34" s="18"/>
       <c r="P34" s="18"/>
       <c r="Q34" s="18"/>
@@ -2354,9 +2354,9 @@
       <c r="AG34" s="18"/>
     </row>
     <row r="35" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A35" s="31"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
       <c r="D35" s="25" t="s">
         <v>23</v>
       </c>
@@ -2364,14 +2364,14 @@
         <v>25</v>
       </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="31"/>
-      <c r="N35" s="31"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="32"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="32"/>
       <c r="O35" s="18"/>
       <c r="P35" s="18"/>
       <c r="Q35" s="18"/>
@@ -2393,9 +2393,9 @@
       <c r="AG35" s="18"/>
     </row>
     <row r="36" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A36" s="31"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
       <c r="D36" s="25" t="s">
         <v>24</v>
       </c>
@@ -2403,14 +2403,14 @@
         <v>25</v>
       </c>
       <c r="F36" s="29"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="31"/>
-      <c r="N36" s="31"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="32"/>
+      <c r="M36" s="32"/>
+      <c r="N36" s="32"/>
       <c r="O36" s="18"/>
       <c r="P36" s="18"/>
       <c r="Q36" s="18"/>
@@ -2432,9 +2432,9 @@
       <c r="AG36" s="18"/>
     </row>
     <row r="37" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
+      <c r="A37" s="33"/>
+      <c r="B37" s="33"/>
+      <c r="C37" s="33"/>
       <c r="D37" s="25" t="s">
         <v>26</v>
       </c>
@@ -2442,14 +2442,14 @@
         <v>25</v>
       </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
-      <c r="I37" s="32"/>
-      <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-      <c r="M37" s="32"/>
-      <c r="N37" s="32"/>
+      <c r="G37" s="33"/>
+      <c r="H37" s="33"/>
+      <c r="I37" s="33"/>
+      <c r="J37" s="33"/>
+      <c r="K37" s="33"/>
+      <c r="L37" s="33"/>
+      <c r="M37" s="33"/>
+      <c r="N37" s="33"/>
       <c r="O37" s="18"/>
       <c r="P37" s="18"/>
       <c r="Q37" s="18"/>
@@ -2506,45 +2506,45 @@
       <c r="AG38" s="18"/>
     </row>
     <row r="39" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A39" s="30">
+      <c r="A39" s="40">
         <v>5</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="34" t="s">
+      <c r="C39" s="42" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E39" s="39" t="s">
+      <c r="E39" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F39" s="40"/>
-      <c r="G39" s="35" t="s">
-        <v>60</v>
+      <c r="F39" s="35"/>
+      <c r="G39" s="31" t="s">
+        <v>59</v>
       </c>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="31" t="s">
         <v>53</v>
       </c>
-      <c r="I39" s="35" t="s">
+      <c r="I39" s="31" t="s">
         <v>54</v>
       </c>
-      <c r="J39" s="35" t="s">
+      <c r="J39" s="31" t="s">
         <v>56</v>
       </c>
-      <c r="K39" s="35" t="s">
+      <c r="K39" s="31" t="s">
         <v>57</v>
       </c>
-      <c r="L39" s="35" t="s">
+      <c r="L39" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="M39" s="35" t="s">
+      <c r="M39" s="31" t="s">
         <v>58</v>
       </c>
-      <c r="N39" s="35" t="s">
-        <v>59</v>
+      <c r="N39" s="31" t="s">
+        <v>61</v>
       </c>
       <c r="O39" s="18"/>
       <c r="P39" s="18"/>
@@ -2567,22 +2567,22 @@
       <c r="AG39" s="18"/>
     </row>
     <row r="40" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A40" s="31"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
+      <c r="A40" s="32"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
       <c r="D40" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E40" s="41"/>
-      <c r="F40" s="42"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
-      <c r="J40" s="31"/>
-      <c r="K40" s="31"/>
-      <c r="L40" s="31"/>
-      <c r="M40" s="31"/>
-      <c r="N40" s="31"/>
+      <c r="E40" s="36"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="32"/>
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="32"/>
+      <c r="L40" s="32"/>
+      <c r="M40" s="32"/>
+      <c r="N40" s="32"/>
       <c r="O40" s="18"/>
       <c r="P40" s="18"/>
       <c r="Q40" s="18"/>
@@ -2604,22 +2604,22 @@
       <c r="AG40" s="18"/>
     </row>
     <row r="41" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A41" s="31"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
+      <c r="A41" s="32"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
       <c r="D41" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
-      <c r="J41" s="31"/>
-      <c r="K41" s="31"/>
-      <c r="L41" s="31"/>
-      <c r="M41" s="31"/>
-      <c r="N41" s="31"/>
+      <c r="E41" s="36"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
+      <c r="J41" s="32"/>
+      <c r="K41" s="32"/>
+      <c r="L41" s="32"/>
+      <c r="M41" s="32"/>
+      <c r="N41" s="32"/>
       <c r="O41" s="18"/>
       <c r="P41" s="18"/>
       <c r="Q41" s="18"/>
@@ -2641,22 +2641,22 @@
       <c r="AG41" s="18"/>
     </row>
     <row r="42" spans="1:33" ht="38" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="32"/>
+      <c r="A42" s="33"/>
+      <c r="B42" s="33"/>
+      <c r="C42" s="33"/>
       <c r="D42" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E42" s="43"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
-      <c r="I42" s="32"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
+      <c r="E42" s="38"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="33"/>
+      <c r="H42" s="33"/>
+      <c r="I42" s="33"/>
+      <c r="J42" s="33"/>
+      <c r="K42" s="33"/>
+      <c r="L42" s="33"/>
+      <c r="M42" s="33"/>
+      <c r="N42" s="33"/>
       <c r="O42" s="18"/>
       <c r="P42" s="18"/>
       <c r="Q42" s="18"/>
@@ -2713,30 +2713,30 @@
       <c r="AG43" s="18"/>
     </row>
     <row r="44" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="30">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="33" t="s">
+      <c r="B44" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C44" s="34" t="s">
+      <c r="C44" s="42" t="s">
         <v>38</v>
       </c>
       <c r="D44" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E44" s="39" t="s">
+      <c r="E44" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F44" s="40"/>
-      <c r="G44" s="35"/>
-      <c r="H44" s="35"/>
-      <c r="I44" s="35"/>
-      <c r="J44" s="35"/>
-      <c r="K44" s="35"/>
-      <c r="L44" s="35"/>
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="31"/>
+      <c r="K44" s="31"/>
+      <c r="L44" s="31"/>
+      <c r="M44" s="31"/>
+      <c r="N44" s="31"/>
       <c r="O44" s="18"/>
       <c r="P44" s="18"/>
       <c r="Q44" s="18"/>
@@ -2758,22 +2758,22 @@
       <c r="AG44" s="18"/>
     </row>
     <row r="45" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A45" s="31"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
+      <c r="A45" s="32"/>
+      <c r="B45" s="32"/>
+      <c r="C45" s="32"/>
       <c r="D45" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="41"/>
-      <c r="F45" s="42"/>
-      <c r="G45" s="31"/>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31"/>
-      <c r="K45" s="31"/>
-      <c r="L45" s="31"/>
-      <c r="M45" s="31"/>
-      <c r="N45" s="31"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="32"/>
+      <c r="H45" s="32"/>
+      <c r="I45" s="32"/>
+      <c r="J45" s="32"/>
+      <c r="K45" s="32"/>
+      <c r="L45" s="32"/>
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
       <c r="O45" s="18"/>
       <c r="P45" s="18"/>
       <c r="Q45" s="18"/>
@@ -2795,22 +2795,22 @@
       <c r="AG45" s="18"/>
     </row>
     <row r="46" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A46" s="31"/>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
+      <c r="A46" s="32"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
       <c r="D46" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E46" s="41"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="31"/>
-      <c r="H46" s="31"/>
-      <c r="I46" s="31"/>
-      <c r="J46" s="31"/>
-      <c r="K46" s="31"/>
-      <c r="L46" s="31"/>
-      <c r="M46" s="31"/>
-      <c r="N46" s="31"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="32"/>
+      <c r="H46" s="32"/>
+      <c r="I46" s="32"/>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
       <c r="O46" s="18"/>
       <c r="P46" s="18"/>
       <c r="Q46" s="18"/>
@@ -2832,22 +2832,22 @@
       <c r="AG46" s="18"/>
     </row>
     <row r="47" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
+      <c r="A47" s="33"/>
+      <c r="B47" s="33"/>
+      <c r="C47" s="33"/>
       <c r="D47" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E47" s="43"/>
-      <c r="F47" s="44"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
-      <c r="I47" s="32"/>
-      <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="32"/>
-      <c r="N47" s="32"/>
+      <c r="E47" s="38"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="33"/>
+      <c r="H47" s="33"/>
+      <c r="I47" s="33"/>
+      <c r="J47" s="33"/>
+      <c r="K47" s="33"/>
+      <c r="L47" s="33"/>
+      <c r="M47" s="33"/>
+      <c r="N47" s="33"/>
       <c r="O47" s="18"/>
       <c r="P47" s="18"/>
       <c r="Q47" s="18"/>
@@ -2904,30 +2904,30 @@
       <c r="AG48" s="18"/>
     </row>
     <row r="49" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A49" s="30">
+      <c r="A49" s="40">
         <v>7</v>
       </c>
-      <c r="B49" s="33" t="s">
+      <c r="B49" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="C49" s="34" t="s">
+      <c r="C49" s="42" t="s">
         <v>40</v>
       </c>
       <c r="D49" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="39" t="s">
+      <c r="E49" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F49" s="40"/>
-      <c r="G49" s="35"/>
-      <c r="H49" s="35"/>
-      <c r="I49" s="35"/>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="35"/>
-      <c r="N49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
+      <c r="I49" s="31"/>
+      <c r="J49" s="31"/>
+      <c r="K49" s="31"/>
+      <c r="L49" s="31"/>
+      <c r="M49" s="31"/>
+      <c r="N49" s="31"/>
       <c r="O49" s="18"/>
       <c r="P49" s="18"/>
       <c r="Q49" s="18"/>
@@ -2949,22 +2949,22 @@
       <c r="AG49" s="18"/>
     </row>
     <row r="50" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A50" s="31"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
+      <c r="A50" s="32"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
       <c r="D50" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="41"/>
-      <c r="F50" s="42"/>
-      <c r="G50" s="31"/>
-      <c r="H50" s="31"/>
-      <c r="I50" s="31"/>
-      <c r="J50" s="31"/>
-      <c r="K50" s="31"/>
-      <c r="L50" s="31"/>
-      <c r="M50" s="31"/>
-      <c r="N50" s="31"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="37"/>
+      <c r="G50" s="32"/>
+      <c r="H50" s="32"/>
+      <c r="I50" s="32"/>
+      <c r="J50" s="32"/>
+      <c r="K50" s="32"/>
+      <c r="L50" s="32"/>
+      <c r="M50" s="32"/>
+      <c r="N50" s="32"/>
       <c r="O50" s="18"/>
       <c r="P50" s="18"/>
       <c r="Q50" s="18"/>
@@ -2986,22 +2986,22 @@
       <c r="AG50" s="18"/>
     </row>
     <row r="51" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="31"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
       <c r="D51" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E51" s="41"/>
-      <c r="F51" s="42"/>
-      <c r="G51" s="31"/>
-      <c r="H51" s="31"/>
-      <c r="I51" s="31"/>
-      <c r="J51" s="31"/>
-      <c r="K51" s="31"/>
-      <c r="L51" s="31"/>
-      <c r="M51" s="31"/>
-      <c r="N51" s="31"/>
+      <c r="E51" s="36"/>
+      <c r="F51" s="37"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
+      <c r="J51" s="32"/>
+      <c r="K51" s="32"/>
+      <c r="L51" s="32"/>
+      <c r="M51" s="32"/>
+      <c r="N51" s="32"/>
       <c r="O51" s="18"/>
       <c r="P51" s="18"/>
       <c r="Q51" s="18"/>
@@ -3023,22 +3023,22 @@
       <c r="AG51" s="18"/>
     </row>
     <row r="52" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="32"/>
+      <c r="A52" s="33"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="33"/>
       <c r="D52" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="E52" s="43"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
-      <c r="I52" s="32"/>
-      <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-      <c r="M52" s="32"/>
-      <c r="N52" s="32"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="33"/>
+      <c r="H52" s="33"/>
+      <c r="I52" s="33"/>
+      <c r="J52" s="33"/>
+      <c r="K52" s="33"/>
+      <c r="L52" s="33"/>
+      <c r="M52" s="33"/>
+      <c r="N52" s="33"/>
       <c r="O52" s="18"/>
       <c r="P52" s="18"/>
       <c r="Q52" s="18"/>
@@ -3095,30 +3095,30 @@
       <c r="AG53" s="18"/>
     </row>
     <row r="54" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A54" s="30">
+      <c r="A54" s="40">
         <v>8</v>
       </c>
-      <c r="B54" s="33" t="s">
+      <c r="B54" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" s="42" t="s">
         <v>42</v>
       </c>
       <c r="D54" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="39" t="s">
+      <c r="E54" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="F54" s="40"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
-      <c r="I54" s="35"/>
-      <c r="J54" s="35"/>
-      <c r="K54" s="35"/>
-      <c r="L54" s="35"/>
-      <c r="M54" s="35"/>
-      <c r="N54" s="35"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="31"/>
+      <c r="K54" s="31"/>
+      <c r="L54" s="31"/>
+      <c r="M54" s="31"/>
+      <c r="N54" s="31"/>
       <c r="O54" s="18"/>
       <c r="P54" s="18"/>
       <c r="Q54" s="18"/>
@@ -3140,22 +3140,22 @@
       <c r="AG54" s="18"/>
     </row>
     <row r="55" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A55" s="31"/>
-      <c r="B55" s="31"/>
-      <c r="C55" s="31"/>
+      <c r="A55" s="32"/>
+      <c r="B55" s="32"/>
+      <c r="C55" s="32"/>
       <c r="D55" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="E55" s="41"/>
-      <c r="F55" s="42"/>
-      <c r="G55" s="31"/>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
-      <c r="K55" s="31"/>
-      <c r="L55" s="31"/>
-      <c r="M55" s="31"/>
-      <c r="N55" s="31"/>
+      <c r="E55" s="36"/>
+      <c r="F55" s="37"/>
+      <c r="G55" s="32"/>
+      <c r="H55" s="32"/>
+      <c r="I55" s="32"/>
+      <c r="J55" s="32"/>
+      <c r="K55" s="32"/>
+      <c r="L55" s="32"/>
+      <c r="M55" s="32"/>
+      <c r="N55" s="32"/>
       <c r="O55" s="18"/>
       <c r="P55" s="18"/>
       <c r="Q55" s="18"/>
@@ -3177,22 +3177,22 @@
       <c r="AG55" s="18"/>
     </row>
     <row r="56" spans="1:33" ht="13" x14ac:dyDescent="0.15">
-      <c r="A56" s="32"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="32"/>
+      <c r="A56" s="33"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="33"/>
       <c r="D56" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="E56" s="43"/>
-      <c r="F56" s="44"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
-      <c r="I56" s="32"/>
-      <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="32"/>
-      <c r="M56" s="32"/>
-      <c r="N56" s="32"/>
+      <c r="E56" s="38"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="33"/>
+      <c r="H56" s="33"/>
+      <c r="I56" s="33"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+      <c r="N56" s="33"/>
       <c r="O56" s="18"/>
       <c r="P56" s="18"/>
       <c r="Q56" s="18"/>
@@ -3249,13 +3249,13 @@
       <c r="AG57" s="18"/>
     </row>
     <row r="58" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A58" s="30">
+      <c r="A58" s="40">
         <v>9</v>
       </c>
-      <c r="B58" s="33" t="s">
+      <c r="B58" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="C58" s="34" t="s">
+      <c r="C58" s="42" t="s">
         <v>44</v>
       </c>
       <c r="D58" s="25" t="s">
@@ -3265,14 +3265,14 @@
         <v>20</v>
       </c>
       <c r="F58" s="29"/>
-      <c r="G58" s="35"/>
-      <c r="H58" s="35"/>
-      <c r="I58" s="35"/>
-      <c r="J58" s="35"/>
-      <c r="K58" s="35"/>
-      <c r="L58" s="35"/>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="31"/>
+      <c r="J58" s="31"/>
+      <c r="K58" s="31"/>
+      <c r="L58" s="31"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="31"/>
       <c r="O58" s="18"/>
       <c r="P58" s="18"/>
       <c r="Q58" s="18"/>
@@ -3294,9 +3294,9 @@
       <c r="AG58" s="18"/>
     </row>
     <row r="59" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A59" s="31"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
+      <c r="A59" s="32"/>
+      <c r="B59" s="32"/>
+      <c r="C59" s="32"/>
       <c r="D59" s="25" t="s">
         <v>21</v>
       </c>
@@ -3304,14 +3304,14 @@
         <v>20</v>
       </c>
       <c r="F59" s="29"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="31"/>
-      <c r="J59" s="31"/>
-      <c r="K59" s="31"/>
-      <c r="L59" s="31"/>
-      <c r="M59" s="31"/>
-      <c r="N59" s="31"/>
+      <c r="G59" s="32"/>
+      <c r="H59" s="32"/>
+      <c r="I59" s="32"/>
+      <c r="J59" s="32"/>
+      <c r="K59" s="32"/>
+      <c r="L59" s="32"/>
+      <c r="M59" s="32"/>
+      <c r="N59" s="32"/>
       <c r="O59" s="18"/>
       <c r="P59" s="18"/>
       <c r="Q59" s="18"/>
@@ -3333,9 +3333,9 @@
       <c r="AG59" s="18"/>
     </row>
     <row r="60" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A60" s="31"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
+      <c r="A60" s="32"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
       <c r="D60" s="25" t="s">
         <v>22</v>
       </c>
@@ -3343,14 +3343,14 @@
         <v>20</v>
       </c>
       <c r="F60" s="29"/>
-      <c r="G60" s="31"/>
-      <c r="H60" s="31"/>
-      <c r="I60" s="31"/>
-      <c r="J60" s="31"/>
-      <c r="K60" s="31"/>
-      <c r="L60" s="31"/>
-      <c r="M60" s="31"/>
-      <c r="N60" s="31"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
+      <c r="I60" s="32"/>
+      <c r="J60" s="32"/>
+      <c r="K60" s="32"/>
+      <c r="L60" s="32"/>
+      <c r="M60" s="32"/>
+      <c r="N60" s="32"/>
       <c r="O60" s="18"/>
       <c r="P60" s="18"/>
       <c r="Q60" s="18"/>
@@ -3372,9 +3372,9 @@
       <c r="AG60" s="18"/>
     </row>
     <row r="61" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A61" s="32"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="32"/>
+      <c r="A61" s="33"/>
+      <c r="B61" s="33"/>
+      <c r="C61" s="33"/>
       <c r="D61" s="25" t="s">
         <v>23</v>
       </c>
@@ -3382,14 +3382,14 @@
         <v>25</v>
       </c>
       <c r="F61" s="29"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
-      <c r="I61" s="32"/>
-      <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-      <c r="M61" s="32"/>
-      <c r="N61" s="32"/>
+      <c r="G61" s="33"/>
+      <c r="H61" s="33"/>
+      <c r="I61" s="33"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="33"/>
+      <c r="N61" s="33"/>
       <c r="O61" s="18"/>
       <c r="P61" s="18"/>
       <c r="Q61" s="18"/>
@@ -3446,13 +3446,13 @@
       <c r="AG62" s="18"/>
     </row>
     <row r="63" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A63" s="30">
+      <c r="A63" s="40">
         <v>10</v>
       </c>
-      <c r="B63" s="33" t="s">
+      <c r="B63" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="C63" s="34" t="s">
+      <c r="C63" s="42" t="s">
         <v>46</v>
       </c>
       <c r="D63" s="25" t="s">
@@ -3462,14 +3462,14 @@
         <v>20</v>
       </c>
       <c r="F63" s="29"/>
-      <c r="G63" s="35"/>
-      <c r="H63" s="35"/>
-      <c r="I63" s="35"/>
-      <c r="J63" s="35"/>
-      <c r="K63" s="35"/>
-      <c r="L63" s="35"/>
-      <c r="M63" s="35"/>
-      <c r="N63" s="35"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="31"/>
+      <c r="K63" s="31"/>
+      <c r="L63" s="31"/>
+      <c r="M63" s="31"/>
+      <c r="N63" s="31"/>
       <c r="O63" s="18"/>
       <c r="P63" s="18"/>
       <c r="Q63" s="18"/>
@@ -3491,9 +3491,9 @@
       <c r="AG63" s="18"/>
     </row>
     <row r="64" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A64" s="31"/>
-      <c r="B64" s="31"/>
-      <c r="C64" s="31"/>
+      <c r="A64" s="32"/>
+      <c r="B64" s="32"/>
+      <c r="C64" s="32"/>
       <c r="D64" s="25" t="s">
         <v>21</v>
       </c>
@@ -3501,14 +3501,14 @@
         <v>20</v>
       </c>
       <c r="F64" s="29"/>
-      <c r="G64" s="31"/>
-      <c r="H64" s="31"/>
-      <c r="I64" s="31"/>
-      <c r="J64" s="31"/>
-      <c r="K64" s="31"/>
-      <c r="L64" s="31"/>
-      <c r="M64" s="31"/>
-      <c r="N64" s="31"/>
+      <c r="G64" s="32"/>
+      <c r="H64" s="32"/>
+      <c r="I64" s="32"/>
+      <c r="J64" s="32"/>
+      <c r="K64" s="32"/>
+      <c r="L64" s="32"/>
+      <c r="M64" s="32"/>
+      <c r="N64" s="32"/>
       <c r="O64" s="18"/>
       <c r="P64" s="18"/>
       <c r="Q64" s="18"/>
@@ -3530,9 +3530,9 @@
       <c r="AG64" s="18"/>
     </row>
     <row r="65" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A65" s="31"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
+      <c r="A65" s="32"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
       <c r="D65" s="25" t="s">
         <v>22</v>
       </c>
@@ -3540,14 +3540,14 @@
         <v>20</v>
       </c>
       <c r="F65" s="29"/>
-      <c r="G65" s="31"/>
-      <c r="H65" s="31"/>
-      <c r="I65" s="31"/>
-      <c r="J65" s="31"/>
-      <c r="K65" s="31"/>
-      <c r="L65" s="31"/>
-      <c r="M65" s="31"/>
-      <c r="N65" s="31"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
+      <c r="I65" s="32"/>
+      <c r="J65" s="32"/>
+      <c r="K65" s="32"/>
+      <c r="L65" s="32"/>
+      <c r="M65" s="32"/>
+      <c r="N65" s="32"/>
       <c r="O65" s="18"/>
       <c r="P65" s="18"/>
       <c r="Q65" s="18"/>
@@ -3569,9 +3569,9 @@
       <c r="AG65" s="18"/>
     </row>
     <row r="66" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="32"/>
+      <c r="A66" s="33"/>
+      <c r="B66" s="33"/>
+      <c r="C66" s="33"/>
       <c r="D66" s="25" t="s">
         <v>23</v>
       </c>
@@ -3579,14 +3579,14 @@
         <v>20</v>
       </c>
       <c r="F66" s="29"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
-      <c r="I66" s="32"/>
-      <c r="J66" s="32"/>
-      <c r="K66" s="32"/>
-      <c r="L66" s="32"/>
-      <c r="M66" s="32"/>
-      <c r="N66" s="32"/>
+      <c r="G66" s="33"/>
+      <c r="H66" s="33"/>
+      <c r="I66" s="33"/>
+      <c r="J66" s="33"/>
+      <c r="K66" s="33"/>
+      <c r="L66" s="33"/>
+      <c r="M66" s="33"/>
+      <c r="N66" s="33"/>
       <c r="O66" s="18"/>
       <c r="P66" s="18"/>
       <c r="Q66" s="18"/>
@@ -3643,13 +3643,13 @@
       <c r="AG67" s="18"/>
     </row>
     <row r="68" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A68" s="30">
+      <c r="A68" s="40">
         <v>11</v>
       </c>
-      <c r="B68" s="33" t="s">
+      <c r="B68" s="41" t="s">
         <v>47</v>
       </c>
-      <c r="C68" s="34" t="s">
+      <c r="C68" s="42" t="s">
         <v>48</v>
       </c>
       <c r="D68" s="25" t="s">
@@ -3659,14 +3659,14 @@
         <v>20</v>
       </c>
       <c r="F68" s="26"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="35"/>
-      <c r="I68" s="35"/>
-      <c r="J68" s="35"/>
-      <c r="K68" s="35"/>
-      <c r="L68" s="35"/>
-      <c r="M68" s="35"/>
-      <c r="N68" s="35"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="31"/>
+      <c r="I68" s="31"/>
+      <c r="J68" s="31"/>
+      <c r="K68" s="31"/>
+      <c r="L68" s="31"/>
+      <c r="M68" s="31"/>
+      <c r="N68" s="31"/>
       <c r="O68" s="18"/>
       <c r="P68" s="18"/>
       <c r="Q68" s="18"/>
@@ -3688,9 +3688,9 @@
       <c r="AG68" s="18"/>
     </row>
     <row r="69" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A69" s="31"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
       <c r="D69" s="25" t="s">
         <v>21</v>
       </c>
@@ -3698,14 +3698,14 @@
         <v>20</v>
       </c>
       <c r="F69" s="26"/>
-      <c r="G69" s="31"/>
-      <c r="H69" s="31"/>
-      <c r="I69" s="31"/>
-      <c r="J69" s="31"/>
-      <c r="K69" s="31"/>
-      <c r="L69" s="31"/>
-      <c r="M69" s="31"/>
-      <c r="N69" s="31"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
+      <c r="J69" s="32"/>
+      <c r="K69" s="32"/>
+      <c r="L69" s="32"/>
+      <c r="M69" s="32"/>
+      <c r="N69" s="32"/>
       <c r="O69" s="18"/>
       <c r="P69" s="18"/>
       <c r="Q69" s="18"/>
@@ -3727,9 +3727,9 @@
       <c r="AG69" s="18"/>
     </row>
     <row r="70" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A70" s="31"/>
-      <c r="B70" s="31"/>
-      <c r="C70" s="31"/>
+      <c r="A70" s="32"/>
+      <c r="B70" s="32"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="25" t="s">
         <v>22</v>
       </c>
@@ -3737,14 +3737,14 @@
         <v>20</v>
       </c>
       <c r="F70" s="26"/>
-      <c r="G70" s="31"/>
-      <c r="H70" s="31"/>
-      <c r="I70" s="31"/>
-      <c r="J70" s="31"/>
-      <c r="K70" s="31"/>
-      <c r="L70" s="31"/>
-      <c r="M70" s="31"/>
-      <c r="N70" s="31"/>
+      <c r="G70" s="32"/>
+      <c r="H70" s="32"/>
+      <c r="I70" s="32"/>
+      <c r="J70" s="32"/>
+      <c r="K70" s="32"/>
+      <c r="L70" s="32"/>
+      <c r="M70" s="32"/>
+      <c r="N70" s="32"/>
       <c r="O70" s="18"/>
       <c r="P70" s="18"/>
       <c r="Q70" s="18"/>
@@ -3766,9 +3766,9 @@
       <c r="AG70" s="18"/>
     </row>
     <row r="71" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="31"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
+      <c r="A71" s="32"/>
+      <c r="B71" s="32"/>
+      <c r="C71" s="32"/>
       <c r="D71" s="25" t="s">
         <v>23</v>
       </c>
@@ -3776,14 +3776,14 @@
         <v>20</v>
       </c>
       <c r="F71" s="26"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="31"/>
+      <c r="G71" s="32"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="32"/>
+      <c r="J71" s="32"/>
+      <c r="K71" s="32"/>
+      <c r="L71" s="32"/>
+      <c r="M71" s="32"/>
+      <c r="N71" s="32"/>
       <c r="O71" s="18"/>
       <c r="P71" s="18"/>
       <c r="Q71" s="18"/>
@@ -3805,9 +3805,9 @@
       <c r="AG71" s="18"/>
     </row>
     <row r="72" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A72" s="31"/>
-      <c r="B72" s="31"/>
-      <c r="C72" s="31"/>
+      <c r="A72" s="32"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
       <c r="D72" s="25" t="s">
         <v>24</v>
       </c>
@@ -3815,14 +3815,14 @@
         <v>20</v>
       </c>
       <c r="F72" s="26"/>
-      <c r="G72" s="31"/>
-      <c r="H72" s="31"/>
-      <c r="I72" s="31"/>
-      <c r="J72" s="31"/>
-      <c r="K72" s="31"/>
-      <c r="L72" s="31"/>
-      <c r="M72" s="31"/>
-      <c r="N72" s="31"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="32"/>
+      <c r="K72" s="32"/>
+      <c r="L72" s="32"/>
+      <c r="M72" s="32"/>
+      <c r="N72" s="32"/>
       <c r="O72" s="18"/>
       <c r="P72" s="18"/>
       <c r="Q72" s="18"/>
@@ -3844,9 +3844,9 @@
       <c r="AG72" s="18"/>
     </row>
     <row r="73" spans="1:33" ht="13" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A73" s="32"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="32"/>
+      <c r="A73" s="33"/>
+      <c r="B73" s="33"/>
+      <c r="C73" s="33"/>
       <c r="D73" s="25" t="s">
         <v>26</v>
       </c>
@@ -3854,14 +3854,14 @@
         <v>20</v>
       </c>
       <c r="F73" s="26"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="32"/>
-      <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-      <c r="M73" s="32"/>
-      <c r="N73" s="32"/>
+      <c r="G73" s="33"/>
+      <c r="H73" s="33"/>
+      <c r="I73" s="33"/>
+      <c r="J73" s="33"/>
+      <c r="K73" s="33"/>
+      <c r="L73" s="33"/>
+      <c r="M73" s="33"/>
+      <c r="N73" s="33"/>
       <c r="O73" s="18"/>
       <c r="P73" s="18"/>
       <c r="Q73" s="18"/>
@@ -37799,33 +37799,81 @@
     </row>
   </sheetData>
   <mergeCells count="126">
-    <mergeCell ref="M49:M52"/>
-    <mergeCell ref="N49:N52"/>
-    <mergeCell ref="E49:F52"/>
-    <mergeCell ref="G49:G52"/>
-    <mergeCell ref="H49:H52"/>
-    <mergeCell ref="I49:I52"/>
-    <mergeCell ref="J49:J52"/>
-    <mergeCell ref="K49:K52"/>
-    <mergeCell ref="L49:L52"/>
-    <mergeCell ref="M44:M47"/>
-    <mergeCell ref="N44:N47"/>
-    <mergeCell ref="E44:F47"/>
-    <mergeCell ref="G44:G47"/>
-    <mergeCell ref="H44:H47"/>
-    <mergeCell ref="I44:I47"/>
-    <mergeCell ref="J44:J47"/>
-    <mergeCell ref="K44:K47"/>
-    <mergeCell ref="L44:L47"/>
-    <mergeCell ref="M39:M42"/>
-    <mergeCell ref="N39:N42"/>
-    <mergeCell ref="E39:F42"/>
-    <mergeCell ref="G39:G42"/>
-    <mergeCell ref="H39:H42"/>
-    <mergeCell ref="I39:I42"/>
-    <mergeCell ref="J39:J42"/>
-    <mergeCell ref="K39:K42"/>
-    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="B15:B22"/>
+    <mergeCell ref="C15:C22"/>
+    <mergeCell ref="A24:A30"/>
+    <mergeCell ref="B24:B30"/>
+    <mergeCell ref="C24:C30"/>
+    <mergeCell ref="B49:B52"/>
+    <mergeCell ref="C49:C52"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="B39:B42"/>
+    <mergeCell ref="C39:C42"/>
+    <mergeCell ref="A44:A47"/>
+    <mergeCell ref="B44:B47"/>
+    <mergeCell ref="C44:C47"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="B63:B66"/>
+    <mergeCell ref="C63:C66"/>
+    <mergeCell ref="A68:A73"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="A54:A56"/>
+    <mergeCell ref="B54:B56"/>
+    <mergeCell ref="C54:C56"/>
+    <mergeCell ref="A58:A61"/>
+    <mergeCell ref="B58:B61"/>
+    <mergeCell ref="C58:C61"/>
+    <mergeCell ref="A63:A66"/>
+    <mergeCell ref="L8:L13"/>
+    <mergeCell ref="M8:M13"/>
+    <mergeCell ref="A1:N1"/>
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="C8:C13"/>
+    <mergeCell ref="G8:G13"/>
+    <mergeCell ref="H8:H13"/>
+    <mergeCell ref="I8:I13"/>
+    <mergeCell ref="N8:N13"/>
+    <mergeCell ref="J8:J13"/>
+    <mergeCell ref="K8:K13"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="L15:L21"/>
+    <mergeCell ref="M15:M21"/>
+    <mergeCell ref="N15:N21"/>
+    <mergeCell ref="G24:G30"/>
+    <mergeCell ref="H24:H30"/>
+    <mergeCell ref="I24:I30"/>
+    <mergeCell ref="J24:J30"/>
+    <mergeCell ref="K24:K30"/>
+    <mergeCell ref="L24:L30"/>
+    <mergeCell ref="M24:M30"/>
+    <mergeCell ref="N24:N30"/>
+    <mergeCell ref="G15:G21"/>
+    <mergeCell ref="H15:H21"/>
+    <mergeCell ref="I15:I21"/>
+    <mergeCell ref="J15:J21"/>
+    <mergeCell ref="K15:K21"/>
+    <mergeCell ref="K32:K37"/>
+    <mergeCell ref="L32:L37"/>
+    <mergeCell ref="M32:M37"/>
+    <mergeCell ref="N32:N37"/>
+    <mergeCell ref="A32:A37"/>
+    <mergeCell ref="B32:B37"/>
+    <mergeCell ref="C32:C37"/>
+    <mergeCell ref="G32:G37"/>
+    <mergeCell ref="H32:H37"/>
+    <mergeCell ref="I32:I37"/>
+    <mergeCell ref="J32:J37"/>
+    <mergeCell ref="M54:M56"/>
+    <mergeCell ref="N54:N56"/>
+    <mergeCell ref="E54:F56"/>
+    <mergeCell ref="G54:G56"/>
+    <mergeCell ref="H54:H56"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="K54:K56"/>
+    <mergeCell ref="L54:L56"/>
     <mergeCell ref="H58:H61"/>
     <mergeCell ref="I58:I61"/>
     <mergeCell ref="J58:J61"/>
@@ -37850,81 +37898,33 @@
     <mergeCell ref="L63:L66"/>
     <mergeCell ref="M63:M66"/>
     <mergeCell ref="N63:N66"/>
-    <mergeCell ref="M54:M56"/>
-    <mergeCell ref="N54:N56"/>
-    <mergeCell ref="E54:F56"/>
-    <mergeCell ref="G54:G56"/>
-    <mergeCell ref="H54:H56"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="J54:J56"/>
-    <mergeCell ref="K54:K56"/>
-    <mergeCell ref="L54:L56"/>
-    <mergeCell ref="K32:K37"/>
-    <mergeCell ref="L32:L37"/>
-    <mergeCell ref="M32:M37"/>
-    <mergeCell ref="N32:N37"/>
-    <mergeCell ref="A32:A37"/>
-    <mergeCell ref="B32:B37"/>
-    <mergeCell ref="C32:C37"/>
-    <mergeCell ref="G32:G37"/>
-    <mergeCell ref="H32:H37"/>
-    <mergeCell ref="I32:I37"/>
-    <mergeCell ref="J32:J37"/>
-    <mergeCell ref="L15:L21"/>
-    <mergeCell ref="M15:M21"/>
-    <mergeCell ref="N15:N21"/>
-    <mergeCell ref="G24:G30"/>
-    <mergeCell ref="H24:H30"/>
-    <mergeCell ref="I24:I30"/>
-    <mergeCell ref="J24:J30"/>
-    <mergeCell ref="K24:K30"/>
-    <mergeCell ref="L24:L30"/>
-    <mergeCell ref="M24:M30"/>
-    <mergeCell ref="N24:N30"/>
-    <mergeCell ref="G15:G21"/>
-    <mergeCell ref="H15:H21"/>
-    <mergeCell ref="I15:I21"/>
-    <mergeCell ref="J15:J21"/>
-    <mergeCell ref="K15:K21"/>
-    <mergeCell ref="L8:L13"/>
-    <mergeCell ref="M8:M13"/>
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="C8:C13"/>
-    <mergeCell ref="G8:G13"/>
-    <mergeCell ref="H8:H13"/>
-    <mergeCell ref="I8:I13"/>
-    <mergeCell ref="N8:N13"/>
-    <mergeCell ref="J8:J13"/>
-    <mergeCell ref="K8:K13"/>
-    <mergeCell ref="B63:B66"/>
-    <mergeCell ref="C63:C66"/>
-    <mergeCell ref="A68:A73"/>
-    <mergeCell ref="B68:B73"/>
-    <mergeCell ref="C68:C73"/>
-    <mergeCell ref="A54:A56"/>
-    <mergeCell ref="B54:B56"/>
-    <mergeCell ref="C54:C56"/>
-    <mergeCell ref="A58:A61"/>
-    <mergeCell ref="B58:B61"/>
-    <mergeCell ref="C58:C61"/>
-    <mergeCell ref="A63:A66"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="B15:B22"/>
-    <mergeCell ref="C15:C22"/>
-    <mergeCell ref="A24:A30"/>
-    <mergeCell ref="B24:B30"/>
-    <mergeCell ref="C24:C30"/>
-    <mergeCell ref="B49:B52"/>
-    <mergeCell ref="C49:C52"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="B39:B42"/>
-    <mergeCell ref="C39:C42"/>
-    <mergeCell ref="A44:A47"/>
-    <mergeCell ref="B44:B47"/>
-    <mergeCell ref="C44:C47"/>
-    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="M39:M42"/>
+    <mergeCell ref="N39:N42"/>
+    <mergeCell ref="E39:F42"/>
+    <mergeCell ref="G39:G42"/>
+    <mergeCell ref="H39:H42"/>
+    <mergeCell ref="I39:I42"/>
+    <mergeCell ref="J39:J42"/>
+    <mergeCell ref="K39:K42"/>
+    <mergeCell ref="L39:L42"/>
+    <mergeCell ref="M44:M47"/>
+    <mergeCell ref="N44:N47"/>
+    <mergeCell ref="E44:F47"/>
+    <mergeCell ref="G44:G47"/>
+    <mergeCell ref="H44:H47"/>
+    <mergeCell ref="I44:I47"/>
+    <mergeCell ref="J44:J47"/>
+    <mergeCell ref="K44:K47"/>
+    <mergeCell ref="L44:L47"/>
+    <mergeCell ref="M49:M52"/>
+    <mergeCell ref="N49:N52"/>
+    <mergeCell ref="E49:F52"/>
+    <mergeCell ref="G49:G52"/>
+    <mergeCell ref="H49:H52"/>
+    <mergeCell ref="I49:I52"/>
+    <mergeCell ref="J49:J52"/>
+    <mergeCell ref="K49:K52"/>
+    <mergeCell ref="L49:L52"/>
   </mergeCells>
   <conditionalFormatting sqref="E2:E1042">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">

</xml_diff>